<commit_message>
changed projects - csv
</commit_message>
<xml_diff>
--- a/data/projects - calculations.xlsx
+++ b/data/projects - calculations.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frac1\Documents\GitHub\SEN9120-Regional energy transition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520CF216-413C-4B4B-979B-1F3E3237B008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F19925-A9AB-415F-9102-CA6F077F5DCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="16788" windowHeight="10728" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Archetypes" sheetId="1" r:id="rId1"/>
-    <sheet name="Offshore wind" sheetId="2" r:id="rId2"/>
+    <sheet name="Offshore wind" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Onshore wind" sheetId="4" r:id="rId3"/>
     <sheet name="Solar Photovoltaic" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -64,17 +64,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="173">
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>cost</t>
-  </si>
-  <si>
-    <t>small offshore wind park</t>
-  </si>
-  <si>
     <t>MW</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
     <t>large solar photovoltaic power station</t>
   </si>
   <si>
-    <t>large offshore wind park</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -444,9 +435,6 @@
     <t>medium solar photovoltaic power station</t>
   </si>
   <si>
-    <t>medium offshore wind park</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -561,30 +549,9 @@
     <t>description</t>
   </si>
   <si>
-    <t>capacity-MW</t>
-  </si>
-  <si>
     <t>References</t>
   </si>
   <si>
-    <t>windpark-small-offshore</t>
-  </si>
-  <si>
-    <t>windpark-large-offshore</t>
-  </si>
-  <si>
-    <t>windpark-medium-offshore</t>
-  </si>
-  <si>
-    <t>windpark-small-onshore</t>
-  </si>
-  <si>
-    <t>windpark-large-onshore</t>
-  </si>
-  <si>
-    <t>windpark-medium-onshore</t>
-  </si>
-  <si>
     <t>solarpark-small</t>
   </si>
   <si>
@@ -594,21 +561,35 @@
     <t>solarpark-medium</t>
   </si>
   <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>s</t>
+    <t>Lead_time_[y]</t>
+  </si>
+  <si>
+    <t>capacity_[MW]</t>
+  </si>
+  <si>
+    <t>Lifespan_[y]</t>
+  </si>
+  <si>
+    <t>solarpark-urban-small</t>
+  </si>
+  <si>
+    <t>windpark-small</t>
+  </si>
+  <si>
+    <t>windpark-medium</t>
+  </si>
+  <si>
+    <t>windpark-large</t>
+  </si>
+  <si>
+    <t>solar panels on urban roofs or parking spaces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -839,43 +820,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -884,11 +862,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+  <cellStyles count="4">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -1125,7 +1102,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1207,7 +1184,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="it-IT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1339,7 +1316,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1186324016"/>
@@ -1401,7 +1378,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1186319856"/>
@@ -1449,7 +1426,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3933,7 +3910,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="it-IT" sz="1100"/>
+                <a:rPr lang="en-US" sz="1100"/>
                 <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
@@ -4052,7 +4029,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="it-IT" sz="1100"/>
+                <a:rPr lang="en-US" sz="1100"/>
                 <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
@@ -4135,7 +4112,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="it-IT" sz="1100"/>
+                <a:rPr lang="en-US" sz="1100"/>
                 <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
@@ -4550,233 +4527,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2AF2E5-58AD-468A-9D04-632533EF6A69}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.21875" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>166</v>
       </c>
       <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
         <v>165</v>
       </c>
-      <c r="D1" t="s">
-        <v>176</v>
-      </c>
       <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="1">
-        <f>'Offshore wind'!I24*C2</f>
-        <v>52480000</v>
-      </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" s="1">
-        <f>'Solar Photovoltaic'!B41*Archetypes!C3</f>
-        <v>10885499.999999998</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>3.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="2">
-        <f>'Onshore wind'!B34*Archetypes!C4</f>
-        <v>4100000</v>
-      </c>
-      <c r="C4">
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" s="1">
-        <f>'Offshore wind'!I24*C5</f>
-        <v>164000000</v>
-      </c>
-      <c r="C5">
-        <v>125</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
       <c r="E5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6" s="1">
-        <f>'Solar Photovoltaic'!B41*Archetypes!C6</f>
-        <v>21045299.999999996</v>
+        <v>163</v>
+      </c>
+      <c r="B6">
+        <v>47</v>
       </c>
       <c r="C6">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" s="2">
-        <f>'Onshore wind'!B34*Archetypes!C7</f>
-        <v>7380000</v>
+        <v>171</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>168</v>
       </c>
-      <c r="B8" s="1">
-        <f>'Offshore wind'!I24*C8</f>
-        <v>695360000</v>
+      <c r="B8">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C8">
-        <v>530</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="1">
-        <f>'Solar Photovoltaic'!B41*Archetypes!C9</f>
-        <v>34107899.999999993</v>
-      </c>
-      <c r="C9">
-        <v>47</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>178</v>
-      </c>
-      <c r="F9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B10" s="2">
-        <f>'Onshore wind'!B34*Archetypes!C10</f>
-        <v>15580000</v>
-      </c>
-      <c r="C10">
-        <v>19</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4810,75 +4709,75 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>752</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>2008</v>
@@ -4887,30 +4786,30 @@
         <v>200000000</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3">
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>2015</v>
@@ -4919,60 +4818,60 @@
         <v>450000000</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4">
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>320</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>2021</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>600</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>2017</v>
@@ -4981,30 +4880,30 @@
         <v>2800000000</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H6">
         <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <v>1996</v>
@@ -5014,30 +4913,30 @@
         <v>23456790.123456787</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8">
         <v>1994</v>
@@ -5047,30 +4946,30 @@
         <v>5605095.5414012736</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H8">
         <v>0.8</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9">
         <v>2008</v>
@@ -5079,143 +4978,143 @@
         <v>350000000</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="A14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I14" t="s">
         <v>140</v>
       </c>
-      <c r="I14" t="s">
-        <v>144</v>
-      </c>
       <c r="J14" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="M14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17">
+      <c r="A15" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15">
         <f>_xlfn.PERCENTILE.EXC(C2:C9,0.25)</f>
         <v>39.75</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f>1600</f>
         <v>1600</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>129</v>
+      <c r="I15" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="J15">
         <v>0.82</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="11">
         <f>H15*J15*1000</f>
         <v>1312000</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>51</v>
+      <c r="L15" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="M15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="19">
+      <c r="B16" s="12"/>
+      <c r="C16" s="17">
         <f>MEDIAN(C2:C9)</f>
         <v>124.5</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22">
+      <c r="A17" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20">
         <f>_xlfn.PERCENTILE.EXC(C2:C9,0.75)</f>
         <v>530</v>
       </c>
       <c r="H17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>133</v>
-      </c>
-      <c r="L17" s="10">
+        <v>129</v>
+      </c>
+      <c r="L17" s="8">
         <f>3588.8*I17^2+3*10^6*I17</f>
         <v>3003588.8</v>
       </c>
       <c r="M17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H19" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L23" s="11"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="I24" s="27">
+      <c r="H24" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="I24" s="25">
         <f>K15</f>
         <v>1312000</v>
       </c>
-      <c r="J24" s="28" t="s">
-        <v>51</v>
+      <c r="J24" s="26" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -5233,7 +5132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A0322F-1D5C-4E90-9801-57AA30159F4F}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -5252,348 +5151,348 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="8">
+        <v>89</v>
+      </c>
+      <c r="C3" s="6">
         <v>2.2999999999999998</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="8">
+        <v>91</v>
+      </c>
+      <c r="C5" s="6">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="8">
+        <v>93</v>
+      </c>
+      <c r="C6" s="6">
         <v>5.2</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="8">
+        <v>95</v>
+      </c>
+      <c r="C7" s="6">
         <v>9.1999999999999993</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="8">
+        <v>97</v>
+      </c>
+      <c r="C8" s="6">
         <v>9.9</v>
       </c>
       <c r="D8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="8">
+        <v>98</v>
+      </c>
+      <c r="C9" s="6">
         <v>9.9</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="8">
+        <v>100</v>
+      </c>
+      <c r="C10" s="6">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="8">
+        <v>101</v>
+      </c>
+      <c r="C11" s="6">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
         <v>102</v>
       </c>
-      <c r="B12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>2.2999999999999998</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="8">
+        <v>104</v>
+      </c>
+      <c r="C13" s="6">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="8">
+        <v>106</v>
+      </c>
+      <c r="C14" s="6">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="8">
+        <v>107</v>
+      </c>
+      <c r="C15" s="6">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
         <v>108</v>
       </c>
-      <c r="B16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="C16" s="6">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="8">
+        <v>109</v>
+      </c>
+      <c r="C17" s="6">
         <v>13.8</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C18" s="8">
+        <v>111</v>
+      </c>
+      <c r="C18" s="6">
         <v>5.88</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="8">
+        <v>113</v>
+      </c>
+      <c r="C19" s="6">
         <v>38.700000000000003</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="8">
+        <v>114</v>
+      </c>
+      <c r="C20" s="6">
         <v>30.1</v>
       </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
         <v>115</v>
       </c>
-      <c r="B21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="C21" s="6">
         <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
-        <v>47</v>
+      <c r="B23" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" s="17">
+      <c r="B24" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="15">
         <f>_xlfn.PERCENTILE.EXC(C1:C20,0.25)</f>
         <v>5.2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="19">
+      <c r="B25" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="17">
         <f>MEDIAN(C2:C21)</f>
         <v>9.1</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C26" s="22">
+      <c r="B26" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="20">
         <f>_xlfn.PERCENTILE.EXC(C2:C21,0.75)</f>
         <v>19.2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
         <v>140</v>
       </c>
-      <c r="B30" t="s">
-        <v>144</v>
-      </c>
       <c r="C30" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -5601,34 +5500,34 @@
         <f>1000</f>
         <v>1000</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>129</v>
+      <c r="B31" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C31">
         <v>0.82</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="11">
         <f>A31*C31*1000</f>
         <v>820000</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>51</v>
+      <c r="E31" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="27" cm="1">
+      <c r="A34" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="25" cm="1">
         <f t="array" ref="B34">Table5[Average cost for offshore wind]</f>
         <v>820000</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>51</v>
+      <c r="C34" s="26" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -5646,8 +5545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2053BEA1-1E26-4AA7-91E9-59408A9B237E}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5665,377 +5564,377 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="6">
+        <v>52</v>
+      </c>
+      <c r="C2" s="4">
         <v>103</v>
       </c>
       <c r="D2">
         <v>320000</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="6">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4">
         <v>54</v>
       </c>
       <c r="D3">
         <v>140000</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4">
         <v>44</v>
       </c>
       <c r="D4">
         <v>170000</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="6">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4">
         <v>40</v>
       </c>
       <c r="D5">
         <v>136000</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="6">
+        <v>60</v>
+      </c>
+      <c r="C6" s="4">
         <v>30</v>
       </c>
       <c r="D6">
         <v>123000</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="6">
+        <v>62</v>
+      </c>
+      <c r="C7" s="4">
         <v>27</v>
       </c>
       <c r="D7">
         <v>76000</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="6">
+        <v>64</v>
+      </c>
+      <c r="C8" s="4">
         <v>15.5</v>
       </c>
       <c r="D8">
         <v>57250</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="6">
+        <v>65</v>
+      </c>
+      <c r="C9" s="4">
         <v>15</v>
       </c>
       <c r="D9">
         <v>125000</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="6">
+        <v>67</v>
+      </c>
+      <c r="C10" s="4">
         <v>15</v>
       </c>
       <c r="D10">
         <v>45000</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="6">
+        <v>69</v>
+      </c>
+      <c r="C11" s="4">
         <v>14</v>
       </c>
       <c r="D11">
         <v>118000</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
-        <v>47</v>
+      <c r="B14" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="17">
+      <c r="B15" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="15">
         <f>_xlfn.PERCENTILE.EXC(C2:C11,0.25)</f>
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="19">
+      <c r="B16" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="17">
         <f>MEDIAN(C2:C11)</f>
         <v>28.5</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="22">
+      <c r="B17" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="20">
         <f>_xlfn.PERCENTILE.EXC(C2:C11,0.75)</f>
         <v>46.5</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="F36" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>145</v>
+      <c r="A36" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>141</v>
       </c>
       <c r="H36" t="s">
-        <v>127</v>
-      </c>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
+        <v>123</v>
+      </c>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B37">
         <f>2.83</f>
         <v>2.83</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D37">
         <v>0.82</v>
       </c>
       <c r="E37" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F37">
         <f>B37*D37</f>
         <v>2.3205999999999998</v>
       </c>
       <c r="G37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H37" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B38">
         <v>0.82</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D38">
         <v>0.82</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" s="7">
+        <v>84</v>
+      </c>
+      <c r="F38" s="5">
         <f t="shared" ref="F38:F39" si="0">B38*D38</f>
         <v>0.67239999999999989</v>
       </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H38" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B39">
         <v>0.95</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D39">
         <v>0.82</v>
       </c>
       <c r="E39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F39" s="7">
+        <v>84</v>
+      </c>
+      <c r="F39" s="5">
         <f t="shared" si="0"/>
         <v>0.77899999999999991</v>
       </c>
       <c r="G39" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="B41" s="30">
+      <c r="A41" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="28">
         <f>AVERAGE(F38:F39)*1000000</f>
         <v>725699.99999999988</v>
       </c>
-      <c r="C41" s="31" t="s">
-        <v>51</v>
+      <c r="C41" s="29" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
consistency between python files and report
</commit_message>
<xml_diff>
--- a/data/projects - calculations.xlsx
+++ b/data/projects - calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frac1\Documents\GitHub\SEN9120-Regional energy transition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F19925-A9AB-415F-9102-CA6F077F5DCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74751DFD-0888-4739-A772-782C5A7111FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="16788" windowHeight="10728" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
+    <workbookView xWindow="-9660" yWindow="2580" windowWidth="16788" windowHeight="10728" firstSheet="2" activeTab="3" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Archetypes" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,13 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Offshore wind'!$C$2:$C$9</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Onshore wind'!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Solar Photovoltaic'!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Onshore wind'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Onshore wind'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Onshore wind'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Onshore wind'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Onshore wind'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Solar Photovoltaic'!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Solar Photovoltaic'!$C$2:$C$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="175">
   <si>
     <t>type</t>
   </si>
@@ -583,6 +589,12 @@
   </si>
   <si>
     <t>solar panels on urban roofs or parking spaces</t>
+  </si>
+  <si>
+    <t>1st quartile</t>
+  </si>
+  <si>
+    <t>3rd quartile</t>
   </si>
 </sst>
 </file>
@@ -826,7 +838,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -861,6 +873,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -1504,7 +1517,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1512,7 +1525,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Wind Onshore capacity</cx:v>
+          <cx:v>Wind Onshore Power Stations</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -1523,7 +1536,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -1532,7 +1545,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Wind Onshore capacity</a:t>
+            <a:t>Wind Onshore Power Stations</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -1547,14 +1560,90 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="1.10000002"/>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1.5"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Distribution</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1300"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Distribution</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Installed capacity [MW]</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1300"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Installed capacity [MW]</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
+        <cx:minorGridlines/>
+        <cx:majorTickMarks type="out"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
     </cx:plotArea>
   </cx:chart>
@@ -1566,38 +1655,61 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
-        <cx:txData>
-          <cx:v>solar Capacity</cx:v>
-        </cx:txData>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0" dirty="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Solar</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="150" baseline="0" dirty="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0" dirty="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>power stations</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
       </cx:tx>
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="all" spc="150" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:rPr>
-            <a:t>solar Capacity</a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
@@ -1609,14 +1721,228 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="1.10000002"/>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1.5"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Distribution</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1300"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Distribution</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Installed capacity [MW]</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1300"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Installed capacity [MW]</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
+        <cx:minorGridlines/>
+        <cx:majorTickMarks type="out"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.6</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Wind Onshore Power Stations</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Wind Onshore Power Stations</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{9D603E98-526B-497C-96AC-D62BDE47A673}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1.5"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Distribution</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1300"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Distribution</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Installed capacity [MW]</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1300"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1300" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Installed capacity [MW]</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:minorGridlines/>
+        <cx:majorTickMarks type="out"/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
     </cx:plotArea>
   </cx:chart>
@@ -1783,6 +2109,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="407">
   <cs:axisTitle>
@@ -2814,7 +3180,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="407">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="374">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2825,7 +3191,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1"/>
+    <cs:defRPr sz="900" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2838,11 +3204,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2890,23 +3256,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2925,6 +3286,9 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2945,11 +3309,6 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:innerShdw blurRad="114300">
-          <a:schemeClr val="phClr"/>
-        </a:innerShdw>
-      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -2981,16 +3340,13 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -3023,8 +3379,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3041,81 +3397,82 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -3127,14 +3484,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-            <a:lumOff val="10000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3143,16 +3500,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -3163,16 +3521,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:leaderLine>
   <cs:legend>
     <cs:lnRef idx="0"/>
@@ -3213,11 +3561,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3245,13 +3593,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:fontRef idx="major">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" cap="all" spc="150"/>
+    <cs:defRPr sz="2000"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3294,11 +3642,11 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="28575">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3328,7 +3676,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="407">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="374">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3339,7 +3687,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1"/>
+    <cs:defRPr sz="900" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -3352,11 +3700,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3404,23 +3752,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -3439,6 +3782,9 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3459,11 +3805,6 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:effectLst>
-        <a:innerShdw blurRad="114300">
-          <a:schemeClr val="phClr"/>
-        </a:innerShdw>
-      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -3495,16 +3836,13 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -3537,8 +3875,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3555,81 +3893,82 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -3641,14 +3980,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-            <a:lumOff val="10000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3657,16 +3996,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -3677,16 +4017,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:leaderLine>
   <cs:legend>
     <cs:lnRef idx="0"/>
@@ -3727,11 +4057,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3759,13 +4089,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:fontRef idx="major">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" cap="all" spc="150"/>
+    <cs:defRPr sz="2000"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3808,11 +4138,507 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="374">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="28575">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3972,7 +4798,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4010,7 +4836,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="6583680" y="0"/>
-              <a:ext cx="3634740" cy="4800600"/>
+              <a:ext cx="3634740" cy="3870960"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4048,15 +4874,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>518160</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -4092,8 +4918,86 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5158740" y="2015490"/>
-              <a:ext cx="5775960" cy="4019550"/>
+              <a:off x="5524500" y="2030730"/>
+              <a:ext cx="3657600" cy="4301490"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>845820</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B91C840-0CE7-4104-BDCB-BB2AF961C7C9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9189720" y="2034540"/>
+              <a:ext cx="3672840" cy="4297680"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4529,8 +5433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2AF2E5-58AD-468A-9D04-632533EF6A69}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4679,6 +5583,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5132,8 +6037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A0322F-1D5C-4E90-9801-57AA30159F4F}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5450,7 +6355,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="21" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="C24" s="15">
         <f>_xlfn.PERCENTILE.EXC(C1:C20,0.25)</f>
@@ -5468,7 +6373,7 @@
     </row>
     <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="23" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="C26" s="20">
         <f>_xlfn.PERCENTILE.EXC(C2:C21,0.75)</f>
@@ -5545,8 +6450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2053BEA1-1E26-4AA7-91E9-59408A9B237E}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5678,7 +6583,7 @@
       <c r="E6" t="s">
         <v>61</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="30" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5789,7 +6694,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="C15" s="15">
         <f>_xlfn.PERCENTILE.EXC(C2:C11,0.25)</f>
@@ -5807,7 +6712,7 @@
     </row>
     <row r="17" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="18" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="C17" s="20">
         <f>_xlfn.PERCENTILE.EXC(C2:C11,0.75)</f>
@@ -5939,11 +6844,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" location="accesstop54" xr:uid="{FECC76B9-6A68-4628-BD8A-3DE0C751893B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementation of update-threshold procedure (to update acceptance thresholds, based on the new installed power at the end of the negotiation)
</commit_message>
<xml_diff>
--- a/data/projects - calculations.xlsx
+++ b/data/projects - calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frac1\Documents\GitHub\ABM_Energy_Transition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9468A05A-1F60-4197-BE8A-D749171B2699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F73103-ED60-4C72-8E43-A32FA16AA5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17400" yWindow="2448" windowWidth="10464" windowHeight="8964" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="10464" windowHeight="8964" xr2:uid="{FFC1AF97-7F4F-45A4-ADD4-756DE35729A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Archetypes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="50" r:id="rId6"/>
+    <pivotCache cacheId="51" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19900,7 +19900,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C5C22EEE-EE31-4B23-89DC-4C6DC5E6F4A7}" name="PivotTable5" cacheId="50" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C5C22EEE-EE31-4B23-89DC-4C6DC5E6F4A7}" name="PivotTable5" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K8:L48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -21500,7 +21500,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>